<commit_message>
MAJ Documentation + Install
</commit_message>
<xml_diff>
--- a/Documentation/NHAIRI_TPI_PlanDeTests_CSHARP.xlsx
+++ b/Documentation/NHAIRI_TPI_PlanDeTests_CSHARP.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>Numéro test</t>
   </si>
@@ -45,10 +45,6 @@
   </si>
   <si>
     <t>L'application se lance sans message d'erreur</t>
-  </si>
-  <si>
-    <t>L'utilisateur crée le compte : "TestRapport" 
-avec le mot de passe "Super"</t>
   </si>
   <si>
     <t>Un message confirme à l'utilsateur que 
@@ -71,14 +67,7 @@
 2. l'onglet musiques s'affiche et présente le résultat de la recherche</t>
   </si>
   <si>
-    <t>L'utilisateur crée une playlist à l'aide du champ se trouvant à coté du bouton "Créer la playlist : "</t>
-  </si>
-  <si>
     <t>Le nom de la playlist doit s'afficher en haut de l'onglet</t>
-  </si>
-  <si>
-    <t>L'utilisateur clique sur le premier morceaux puis 
-clique sur "Ajouter aux favoris" et "Ajouter à la playlist:"</t>
   </si>
   <si>
     <t>L'utilisateur clique sur l'onglet "Favoris"</t>
@@ -135,6 +124,17 @@
   </si>
   <si>
     <t>L'application se ferme sans messages d'erreur</t>
+  </si>
+  <si>
+    <t>L'utilisateur clique sur le premier morceau puis 
+clique sur "Ajouter aux favoris" et "Ajouter à la playlist:"</t>
+  </si>
+  <si>
+    <t>L'utilisateur clique sur "Inscription" crée le compte : "TestRapport" 
+avec le mot de passe "Super"</t>
+  </si>
+  <si>
+    <t>L'utilisateur crée une playlist à l'aide du champ se trouvant à coté du bouton "Créer la playlist : " avec comme nom : "Playlist Test"</t>
   </si>
 </sst>
 </file>
@@ -344,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -403,6 +403,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -685,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,10 +741,10 @@
         <v>4</v>
       </c>
       <c r="E5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>7</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -748,10 +755,10 @@
         <v>4</v>
       </c>
       <c r="E6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>9</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -762,10 +769,10 @@
         <v>4</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -776,10 +783,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>11</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="9" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -790,10 +797,10 @@
         <v>4</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -804,10 +811,10 @@
         <v>4</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -818,10 +825,10 @@
         <v>4</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -832,10 +839,10 @@
         <v>4</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -846,10 +853,10 @@
         <v>4</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -860,10 +867,10 @@
         <v>4</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -874,10 +881,10 @@
         <v>4</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -888,10 +895,10 @@
         <v>4</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -902,175 +909,115 @@
         <v>4</v>
       </c>
       <c r="E17" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="6">
+        <v>15</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F18" s="19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="4">
-        <v>15</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="4">
-        <v>16</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12"/>
-    </row>
-    <row r="20" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="4">
-        <v>17</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="12"/>
-    </row>
-    <row r="21" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="4">
-        <v>18</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="4">
-        <v>19</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="12"/>
-    </row>
-    <row r="23" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="4">
-        <v>20</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="12"/>
-    </row>
-    <row r="24" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="4">
-        <v>21</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="12"/>
-    </row>
-    <row r="25" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="4">
-        <v>22</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="12"/>
-    </row>
-    <row r="26" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="4">
-        <v>23</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="12"/>
-    </row>
-    <row r="27" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="4">
-        <v>24</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="12"/>
-    </row>
-    <row r="28" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="4">
-        <v>25</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" s="11"/>
-      <c r="F28" s="12"/>
-    </row>
-    <row r="29" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="4">
-        <v>26</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E29" s="11"/>
-      <c r="F29" s="12"/>
-    </row>
-    <row r="30" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="4">
-        <v>27</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="12"/>
-    </row>
-    <row r="31" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="4">
-        <v>28</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="11"/>
-      <c r="F31" s="12"/>
-    </row>
-    <row r="32" spans="3:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="4">
-        <v>29</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="11"/>
-      <c r="F32" s="12"/>
-    </row>
-    <row r="33" spans="3:6" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="6">
-        <v>30</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E33" s="18"/>
-      <c r="F33" s="19"/>
+    <row r="19" spans="3:6" s="22" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+    </row>
+    <row r="20" spans="3:6" s="22" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+    </row>
+    <row r="21" spans="3:6" s="22" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+    </row>
+    <row r="22" spans="3:6" s="22" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+    </row>
+    <row r="23" spans="3:6" s="22" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+    </row>
+    <row r="24" spans="3:6" s="22" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+    </row>
+    <row r="25" spans="3:6" s="22" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+    </row>
+    <row r="26" spans="3:6" s="22" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+    </row>
+    <row r="27" spans="3:6" s="22" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+    </row>
+    <row r="28" spans="3:6" s="22" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+    </row>
+    <row r="29" spans="3:6" s="22" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+    </row>
+    <row r="30" spans="3:6" s="22" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+    </row>
+    <row r="31" spans="3:6" s="22" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+    </row>
+    <row r="32" spans="3:6" s="22" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+    </row>
+    <row r="33" spans="3:6" s="22" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>